<commit_message>
add columns for excel test cases
</commit_message>
<xml_diff>
--- a/tests/excel/shuihudata.xlsx
+++ b/tests/excel/shuihudata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\f2t\tests\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0F3DC1-70AB-439C-A251-6D5BDEAD355B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B976946B-BCCE-4AF4-BE14-A691B4C665EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="334">
   <si>
     <t>座次</t>
   </si>
@@ -1027,15 +1027,23 @@
   </si>
   <si>
     <t>段景住</t>
+  </si>
+  <si>
+    <t>年月日</t>
+  </si>
+  <si>
+    <t>时分秒</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="177" formatCode="0_ "/>
-    <numFmt numFmtId="180" formatCode="0.000000_ "/>
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="0_ "/>
+    <numFmt numFmtId="177" formatCode="0.000000_ "/>
+    <numFmt numFmtId="178" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1623,7 +1631,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1633,7 +1641,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1686,16 +1700,13 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="177" formatCode="0_ "/>
+      <numFmt numFmtId="27" formatCode="yyyy/m/d\ h:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="180" formatCode="0.000000_ "/>
+      <numFmt numFmtId="176" formatCode="0_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="0_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm"/>
+      <numFmt numFmtId="177" formatCode="0.000000_ "/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1705,6 +1716,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0_ "/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1740,14 +1754,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="shuihudata" displayName="shuihudata" ref="A1:H109" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H109" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="座次" queryTableFieldId="1" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="星宿" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="诨名" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="姓名" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="座次" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="星宿" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="诨名" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="姓名" queryTableFieldId="4" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="布尔" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="浮点" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="整数" queryTableFieldId="7" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="日期" queryTableFieldId="8" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="浮点" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="整数" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="日期" queryTableFieldId="8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2050,10 +2064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2065,9 +2079,11 @@
     <col min="6" max="6" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2092,8 +2108,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="J1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2118,8 +2140,14 @@
       <c r="H2" s="1">
         <v>44157.768020833333</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="6">
+        <v>42200</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0.96351851851851855</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2144,8 +2172,14 @@
       <c r="H3" s="1">
         <v>44157.439710648148</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="6">
+        <v>30025</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.54396990740740736</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2170,8 +2204,14 @@
       <c r="H4" s="1">
         <v>44157.49732638889</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="6">
+        <v>35018</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.31486111111111109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2196,8 +2236,14 @@
       <c r="H5" s="1">
         <v>44157.320474537039</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="6">
+        <v>27628</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.49040509259259257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2222,8 +2268,14 @@
       <c r="H6" s="1">
         <v>44157.434050925927</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="6">
+        <v>35776</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.99633101851851846</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2248,8 +2300,14 @@
       <c r="H7" s="1">
         <v>44157.805486111109</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="6">
+        <v>25821</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.80730324074074078</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2274,8 +2332,14 @@
       <c r="H8" s="1">
         <v>44157.63003472222</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="6">
+        <v>38082</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0.46479166666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2300,8 +2364,14 @@
       <c r="H9" s="1">
         <v>44157.743263888886</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="6">
+        <v>39122</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0.89864583333333337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2326,8 +2396,14 @@
       <c r="H10" s="1">
         <v>44157.88045138889</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="6">
+        <v>40722</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0.81950231481481484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2352,8 +2428,14 @@
       <c r="H11" s="1">
         <v>44157.683321759258</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="6">
+        <v>26380</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0.76891203703703703</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2378,8 +2460,14 @@
       <c r="H12" s="1">
         <v>44156.967789351853</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="6">
+        <v>44751</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0.21729166666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2404,8 +2492,14 @@
       <c r="H13" s="1">
         <v>44157.883125</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="6">
+        <v>27822</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0.85788194444444443</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2430,8 +2524,14 @@
       <c r="H14" s="1">
         <v>44157.401400462964</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="6">
+        <v>27794</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0.56891203703703708</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2456,8 +2556,14 @@
       <c r="H15" s="1">
         <v>44157.660752314812</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="6">
+        <v>40296</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0.39291666666666669</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2482,8 +2588,14 @@
       <c r="H16" s="1">
         <v>44157.177210648151</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="6">
+        <v>31931</v>
+      </c>
+      <c r="J16" s="5">
+        <v>5.917824074074074E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2508,8 +2620,14 @@
       <c r="H17" s="1">
         <v>44157.255046296297</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="6">
+        <v>29507</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0.19798611111111111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2534,8 +2652,14 @@
       <c r="H18" s="1">
         <v>44157.026608796295</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="6">
+        <v>44521</v>
+      </c>
+      <c r="J18" s="5">
+        <v>9.0636574074074078E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2560,8 +2684,14 @@
       <c r="H19" s="1">
         <v>44157.396805555552</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="6">
+        <v>36949</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0.14577546296296295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2586,8 +2716,14 @@
       <c r="H20" s="1">
         <v>44157.434328703705</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="6">
+        <v>27573</v>
+      </c>
+      <c r="J20" s="5">
+        <v>0.97349537037037037</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2612,8 +2748,14 @@
       <c r="H21" s="1">
         <v>44157.153587962966</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="6">
+        <v>36442</v>
+      </c>
+      <c r="J21" s="5">
+        <v>0.79398148148148151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2638,8 +2780,14 @@
       <c r="H22" s="1">
         <v>44157.18922453704</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="6">
+        <v>44126</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0.57502314814814814</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2664,8 +2812,14 @@
       <c r="H23" s="1">
         <v>44157.636921296296</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="6">
+        <v>26882</v>
+      </c>
+      <c r="J23" s="5">
+        <v>0.55196759259259254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2690,8 +2844,14 @@
       <c r="H24" s="1">
         <v>44157.609351851854</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="6">
+        <v>32395</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0.71467592592592588</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2716,8 +2876,14 @@
       <c r="H25" s="1">
         <v>44157.562557870369</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="6">
+        <v>34900</v>
+      </c>
+      <c r="J25" s="5">
+        <v>8.8206018518518517E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2742,8 +2908,14 @@
       <c r="H26" s="1">
         <v>44157.554976851854</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="6">
+        <v>34293</v>
+      </c>
+      <c r="J26" s="5">
+        <v>0.89177083333333329</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2768,8 +2940,14 @@
       <c r="H27" s="1">
         <v>44157.263368055559</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="6">
+        <v>31536</v>
+      </c>
+      <c r="J27" s="5">
+        <v>0.90598379629629633</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2794,8 +2972,14 @@
       <c r="H28" s="1">
         <v>44157.863159722219</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="6">
+        <v>39996</v>
+      </c>
+      <c r="J28" s="5">
+        <v>7.1157407407407405E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2820,8 +3004,14 @@
       <c r="H29" s="1">
         <v>44157.642118055555</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="6">
+        <v>27097</v>
+      </c>
+      <c r="J29" s="5">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2846,8 +3036,14 @@
       <c r="H30" s="1">
         <v>44157.385833333334</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="6">
+        <v>31758</v>
+      </c>
+      <c r="J30" s="5">
+        <v>0.57815972222222223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2872,8 +3068,14 @@
       <c r="H31" s="1">
         <v>44157.572372685187</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="6">
+        <v>34211</v>
+      </c>
+      <c r="J31" s="5">
+        <v>0.55518518518518523</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2898,8 +3100,14 @@
       <c r="H32" s="1">
         <v>44157.536215277774</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="6">
+        <v>42977</v>
+      </c>
+      <c r="J32" s="5">
+        <v>0.3036226851851852</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2924,8 +3132,14 @@
       <c r="H33" s="1">
         <v>44157.895925925928</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="6">
+        <v>28454</v>
+      </c>
+      <c r="J33" s="5">
+        <v>0.43074074074074076</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2950,8 +3164,14 @@
       <c r="H34" s="1">
         <v>44157.364988425928</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="6">
+        <v>32770</v>
+      </c>
+      <c r="J34" s="5">
+        <v>0.17023148148148148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2976,8 +3196,14 @@
       <c r="H35" s="1">
         <v>44157.894942129627</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="6">
+        <v>29880</v>
+      </c>
+      <c r="J35" s="5">
+        <v>0.2457175925925926</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3002,8 +3228,14 @@
       <c r="H36" s="1">
         <v>44157.470821759256</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="6">
+        <v>25729</v>
+      </c>
+      <c r="J36" s="5">
+        <v>0.72164351851851849</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3028,8 +3260,14 @@
       <c r="H37" s="1">
         <v>44157.42150462963</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="6">
+        <v>43195</v>
+      </c>
+      <c r="J37" s="5">
+        <v>0.596099537037037</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3054,8 +3292,14 @@
       <c r="H38" s="1">
         <v>44157.7812962963</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="6">
+        <v>28961</v>
+      </c>
+      <c r="J38" s="5">
+        <v>0.33002314814814815</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3080,8 +3324,14 @@
       <c r="H39" s="1">
         <v>44157.536215277774</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="6">
+        <v>34737</v>
+      </c>
+      <c r="J39" s="5">
+        <v>7.3831018518518518E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3106,8 +3356,14 @@
       <c r="H40" s="1">
         <v>44157.529224537036</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="6">
+        <v>26219</v>
+      </c>
+      <c r="J40" s="5">
+        <v>0.24888888888888888</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3132,8 +3388,14 @@
       <c r="H41" s="1">
         <v>44157.221250000002</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="6">
+        <v>43600</v>
+      </c>
+      <c r="J41" s="5">
+        <v>0.21012731481481481</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3158,8 +3420,14 @@
       <c r="H42" s="1">
         <v>44157.57571759259</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="6">
+        <v>36152</v>
+      </c>
+      <c r="J42" s="5">
+        <v>0.62944444444444447</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3184,8 +3452,14 @@
       <c r="H43" s="1">
         <v>44157.293217592596</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="6">
+        <v>32884</v>
+      </c>
+      <c r="J43" s="5">
+        <v>0.1265162037037037</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3210,8 +3484,14 @@
       <c r="H44" s="1">
         <v>44157.230011574073</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="6">
+        <v>28830</v>
+      </c>
+      <c r="J44" s="5">
+        <v>0.12484953703703704</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3236,8 +3516,14 @@
       <c r="H45" s="1">
         <v>44157.796006944445</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="6">
+        <v>41621</v>
+      </c>
+      <c r="J45" s="5">
+        <v>0.38263888888888886</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3262,8 +3548,14 @@
       <c r="H46" s="1">
         <v>44157.617754629631</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="6">
+        <v>26778</v>
+      </c>
+      <c r="J46" s="5">
+        <v>0.5158449074074074</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3288,8 +3580,14 @@
       <c r="H47" s="1">
         <v>44157.536493055559</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="6">
+        <v>40142</v>
+      </c>
+      <c r="J47" s="5">
+        <v>0.97865740740740736</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3314,8 +3612,14 @@
       <c r="H48" s="1">
         <v>44157.840428240743</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="6">
+        <v>28624</v>
+      </c>
+      <c r="J48" s="5">
+        <v>0.27199074074074076</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3340,8 +3644,14 @@
       <c r="H49" s="1">
         <v>44157.872256944444</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="6">
+        <v>34116</v>
+      </c>
+      <c r="J49" s="5">
+        <v>0.19340277777777778</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3366,8 +3676,14 @@
       <c r="H50" s="1">
         <v>44157.345462962963</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="6">
+        <v>34726</v>
+      </c>
+      <c r="J50" s="5">
+        <v>0.42298611111111112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3392,8 +3708,14 @@
       <c r="H51" s="1">
         <v>44156.962361111109</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="6">
+        <v>37126</v>
+      </c>
+      <c r="J51" s="5">
+        <v>0.77229166666666671</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3418,8 +3740,14 @@
       <c r="H52" s="1">
         <v>44157.895601851851</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="6">
+        <v>40012</v>
+      </c>
+      <c r="J52" s="5">
+        <v>0.19524305555555554</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3444,8 +3772,14 @@
       <c r="H53" s="1">
         <v>44156.985659722224</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="6">
+        <v>36207</v>
+      </c>
+      <c r="J53" s="5">
+        <v>0.30422453703703706</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -3470,8 +3804,14 @@
       <c r="H54" s="1">
         <v>44157.31722222222</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="6">
+        <v>40759</v>
+      </c>
+      <c r="J54" s="5">
+        <v>0.59119212962962964</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -3496,8 +3836,14 @@
       <c r="H55" s="1">
         <v>44157.230798611112</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="6">
+        <v>27768</v>
+      </c>
+      <c r="J55" s="5">
+        <v>0.59018518518518515</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -3522,8 +3868,14 @@
       <c r="H56" s="1">
         <v>44157.237349537034</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="6">
+        <v>39862</v>
+      </c>
+      <c r="J56" s="5">
+        <v>0.41554398148148147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -3548,8 +3900,14 @@
       <c r="H57" s="1">
         <v>44157.24150462963</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="6">
+        <v>36410</v>
+      </c>
+      <c r="J57" s="5">
+        <v>0.52429398148148143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -3574,8 +3932,14 @@
       <c r="H58" s="1">
         <v>44157.636932870373</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="6">
+        <v>29648</v>
+      </c>
+      <c r="J58" s="5">
+        <v>0.64682870370370371</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -3600,8 +3964,14 @@
       <c r="H59" s="1">
         <v>44157.440833333334</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="6">
+        <v>31261</v>
+      </c>
+      <c r="J59" s="5">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -3626,8 +3996,14 @@
       <c r="H60" s="1">
         <v>44157.609212962961</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="6">
+        <v>37319</v>
+      </c>
+      <c r="J60" s="5">
+        <v>0.20734953703703704</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -3652,8 +4028,14 @@
       <c r="H61" s="1">
         <v>44156.942372685182</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="6">
+        <v>31018</v>
+      </c>
+      <c r="J61" s="5">
+        <v>0.31692129629629628</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -3678,8 +4060,14 @@
       <c r="H62" s="1">
         <v>44156.987997685188</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="6">
+        <v>34127</v>
+      </c>
+      <c r="J62" s="5">
+        <v>0.89378472222222227</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -3704,8 +4092,14 @@
       <c r="H63" s="1">
         <v>44157.302118055559</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="6">
+        <v>40086</v>
+      </c>
+      <c r="J63" s="5">
+        <v>0.85995370370370372</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -3730,8 +4124,14 @@
       <c r="H64" s="1">
         <v>44157.905405092592</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="6">
+        <v>27201</v>
+      </c>
+      <c r="J64" s="5">
+        <v>0.78949074074074077</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -3756,8 +4156,14 @@
       <c r="H65" s="1">
         <v>44157.905532407407</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="6">
+        <v>25996</v>
+      </c>
+      <c r="J65" s="5">
+        <v>0.32135416666666666</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -3782,8 +4188,14 @@
       <c r="H66" s="1">
         <v>44157.095451388886</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="6">
+        <v>28947</v>
+      </c>
+      <c r="J66" s="5">
+        <v>0.62483796296296301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -3808,8 +4220,14 @@
       <c r="H67" s="1">
         <v>44157.705405092594</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="6">
+        <v>43429</v>
+      </c>
+      <c r="J67" s="5">
+        <v>0.72317129629629628</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -3834,8 +4252,14 @@
       <c r="H68" s="1">
         <v>44157.889525462961</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="6">
+        <v>26122</v>
+      </c>
+      <c r="J68" s="5">
+        <v>0.13605324074074074</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -3860,8 +4284,14 @@
       <c r="H69" s="1">
         <v>44156.973703703705</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="6">
+        <v>36367</v>
+      </c>
+      <c r="J69" s="5">
+        <v>0.14534722222222221</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -3886,8 +4316,14 @@
       <c r="H70" s="1">
         <v>44157.743634259263</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="6">
+        <v>27678</v>
+      </c>
+      <c r="J70" s="5">
+        <v>0.13314814814814815</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -3912,8 +4348,14 @@
       <c r="H71" s="1">
         <v>44157.758900462963</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="6">
+        <v>29781</v>
+      </c>
+      <c r="J71" s="5">
+        <v>0.83187500000000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -3938,8 +4380,14 @@
       <c r="H72" s="1">
         <v>44157.84</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="6">
+        <v>29983</v>
+      </c>
+      <c r="J72" s="5">
+        <v>0.60543981481481479</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -3964,8 +4412,14 @@
       <c r="H73" s="1">
         <v>44157.632557870369</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="6">
+        <v>31983</v>
+      </c>
+      <c r="J73" s="5">
+        <v>0.78482638888888889</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -3990,8 +4444,14 @@
       <c r="H74" s="1">
         <v>44157.883657407408</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="6">
+        <v>33591</v>
+      </c>
+      <c r="J74" s="5">
+        <v>9.7222222222222219E-4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -4016,8 +4476,14 @@
       <c r="H75" s="1">
         <v>44157.484861111108</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="6">
+        <v>34797</v>
+      </c>
+      <c r="J75" s="5">
+        <v>0.91938657407407409</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -4042,8 +4508,14 @@
       <c r="H76" s="1">
         <v>44157.319027777776</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="6">
+        <v>42853</v>
+      </c>
+      <c r="J76" s="5">
+        <v>0.13945601851851852</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -4068,8 +4540,14 @@
       <c r="H77" s="1">
         <v>44156.986493055556</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="6">
+        <v>35476</v>
+      </c>
+      <c r="J77" s="5">
+        <v>0.14993055555555557</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -4094,8 +4572,14 @@
       <c r="H78" s="1">
         <v>44157.066504629627</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="6">
+        <v>34349</v>
+      </c>
+      <c r="J78" s="5">
+        <v>0.74177083333333338</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -4120,8 +4604,14 @@
       <c r="H79" s="1">
         <v>44157.466898148145</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="6">
+        <v>32600</v>
+      </c>
+      <c r="J79" s="5">
+        <v>0.46822916666666664</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -4146,8 +4636,14 @@
       <c r="H80" s="1">
         <v>44157.299988425926</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="6">
+        <v>31183</v>
+      </c>
+      <c r="J80" s="5">
+        <v>0.32101851851851854</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -4172,8 +4668,14 @@
       <c r="H81" s="1">
         <v>44157.423194444447</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="6">
+        <v>37078</v>
+      </c>
+      <c r="J81" s="5">
+        <v>0.92254629629629625</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -4198,8 +4700,14 @@
       <c r="H82" s="1">
         <v>44157.704710648148</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="6">
+        <v>36644</v>
+      </c>
+      <c r="J82" s="5">
+        <v>0.59126157407407409</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -4224,8 +4732,14 @@
       <c r="H83" s="1">
         <v>44157.552916666667</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="6">
+        <v>32898</v>
+      </c>
+      <c r="J83" s="5">
+        <v>0.41858796296296297</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -4250,8 +4764,14 @@
       <c r="H84" s="1">
         <v>44157.756180555552</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="6">
+        <v>29686</v>
+      </c>
+      <c r="J84" s="5">
+        <v>0.15929398148148149</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -4276,8 +4796,14 @@
       <c r="H85" s="1">
         <v>44157.453217592592</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="6">
+        <v>43602</v>
+      </c>
+      <c r="J85" s="5">
+        <v>0.4221759259259259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -4302,8 +4828,14 @@
       <c r="H86" s="1">
         <v>44157.169108796297</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="6">
+        <v>26841</v>
+      </c>
+      <c r="J86" s="5">
+        <v>6.293981481481481E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -4328,8 +4860,14 @@
       <c r="H87" s="1">
         <v>44157.890555555554</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="6">
+        <v>26565</v>
+      </c>
+      <c r="J87" s="5">
+        <v>0.85739583333333336</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -4354,8 +4892,14 @@
       <c r="H88" s="1">
         <v>44157.360266203701</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="6">
+        <v>28404</v>
+      </c>
+      <c r="J88" s="5">
+        <v>0.42969907407407409</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -4380,8 +4924,14 @@
       <c r="H89" s="1">
         <v>44157.026099537034</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="6">
+        <v>34643</v>
+      </c>
+      <c r="J89" s="5">
+        <v>3.7951388888888889E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -4406,8 +4956,14 @@
       <c r="H90" s="1">
         <v>44157.296516203707</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="6">
+        <v>26083</v>
+      </c>
+      <c r="J90" s="5">
+        <v>0.2192361111111111</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -4432,8 +4988,14 @@
       <c r="H91" s="1">
         <v>44157.429618055554</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="6">
+        <v>26424</v>
+      </c>
+      <c r="J91" s="5">
+        <v>3.8078703703703703E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -4458,8 +5020,14 @@
       <c r="H92" s="1">
         <v>44157.488206018519</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="6">
+        <v>39631</v>
+      </c>
+      <c r="J92" s="5">
+        <v>0.97927083333333331</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -4484,8 +5052,14 @@
       <c r="H93" s="1">
         <v>44157.858634259261</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="6">
+        <v>35031</v>
+      </c>
+      <c r="J93" s="5">
+        <v>0.58603009259259264</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -4510,8 +5084,14 @@
       <c r="H94" s="1">
         <v>44157.341203703705</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="6">
+        <v>39206</v>
+      </c>
+      <c r="J94" s="5">
+        <v>0.32078703703703704</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -4536,8 +5116,14 @@
       <c r="H95" s="1">
         <v>44157.438379629632</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="6">
+        <v>38249</v>
+      </c>
+      <c r="J95" s="5">
+        <v>1.1446759259259259E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -4562,8 +5148,14 @@
       <c r="H96" s="1">
         <v>44157.721967592595</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="6">
+        <v>36749</v>
+      </c>
+      <c r="J96" s="5">
+        <v>0.9427430555555556</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -4588,8 +5180,14 @@
       <c r="H97" s="1">
         <v>44157.313275462962</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="6">
+        <v>39107</v>
+      </c>
+      <c r="J97" s="5">
+        <v>6.6817129629629629E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -4614,8 +5212,14 @@
       <c r="H98" s="1">
         <v>44157.625196759262</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="6">
+        <v>44055</v>
+      </c>
+      <c r="J98" s="5">
+        <v>0.37190972222222224</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -4640,8 +5244,14 @@
       <c r="H99" s="1">
         <v>44157.002210648148</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="6">
+        <v>35105</v>
+      </c>
+      <c r="J99" s="5">
+        <v>0.18274305555555556</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -4666,8 +5276,14 @@
       <c r="H100" s="1">
         <v>44157.179027777776</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="6">
+        <v>39973</v>
+      </c>
+      <c r="J100" s="5">
+        <v>0.4244560185185185</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -4692,8 +5308,14 @@
       <c r="H101" s="1">
         <v>44157.013356481482</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="6">
+        <v>37212</v>
+      </c>
+      <c r="J101" s="5">
+        <v>0.73589120370370376</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -4718,8 +5340,14 @@
       <c r="H102" s="1">
         <v>44157.495787037034</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="6">
+        <v>37083</v>
+      </c>
+      <c r="J102" s="5">
+        <v>0.57832175925925922</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -4744,8 +5372,14 @@
       <c r="H103" s="1">
         <v>44157.041504629633</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="6">
+        <v>37792</v>
+      </c>
+      <c r="J103" s="5">
+        <v>0.83019675925925929</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -4770,8 +5404,14 @@
       <c r="H104" s="1">
         <v>44156.973761574074</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="6">
+        <v>32385</v>
+      </c>
+      <c r="J104" s="5">
+        <v>0.31170138888888888</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -4796,8 +5436,14 @@
       <c r="H105" s="1">
         <v>44157.741608796299</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="6">
+        <v>39678</v>
+      </c>
+      <c r="J105" s="5">
+        <v>0.24373842592592593</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -4822,8 +5468,14 @@
       <c r="H106" s="1">
         <v>44157.245162037034</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="6">
+        <v>31973</v>
+      </c>
+      <c r="J106" s="5">
+        <v>0.8989583333333333</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -4848,8 +5500,14 @@
       <c r="H107" s="1">
         <v>44157.171423611115</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="6">
+        <v>33707</v>
+      </c>
+      <c r="J107" s="5">
+        <v>0.62105324074074075</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -4874,8 +5532,14 @@
       <c r="H108" s="1">
         <v>44157.230995370373</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="6">
+        <v>32843</v>
+      </c>
+      <c r="J108" s="5">
+        <v>4.0254629629629626E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -4899,6 +5563,12 @@
       </c>
       <c r="H109" s="1">
         <v>44156.993622685186</v>
+      </c>
+      <c r="I109" s="6">
+        <v>39061</v>
+      </c>
+      <c r="J109" s="5">
+        <v>0.33899305555555553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>